<commit_message>
Registeration of user using csv completed
</commit_message>
<xml_diff>
--- a/excel/RegisterData.xlsx
+++ b/excel/RegisterData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>FirstName</t>
   </si>
@@ -50,6 +50,30 @@
   </si>
   <si>
     <t>Khalti</t>
+  </si>
+  <si>
+    <t>sonytuladhar25@gmail.com</t>
+  </si>
+  <si>
+    <t>Khalti1</t>
+  </si>
+  <si>
+    <t>sonytuladhar26@gmail.com</t>
+  </si>
+  <si>
+    <t>Khalti2</t>
+  </si>
+  <si>
+    <t>sonytuladhar27@gmail.com</t>
+  </si>
+  <si>
+    <t>Khalti3</t>
+  </si>
+  <si>
+    <t>sonytuladhar28@gmail.com</t>
+  </si>
+  <si>
+    <t>Khalti4</t>
   </si>
 </sst>
 </file>
@@ -366,6 +390,122 @@
         <v>7.6697669E7</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1994.0</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1">
+        <v>7.6697669E7</v>
+      </c>
+      <c r="I3" s="1">
+        <v>7.6697669E7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>12.0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1994.0</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="1">
+        <v>7.6697669E7</v>
+      </c>
+      <c r="I4" s="1">
+        <v>7.6697669E7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>13.0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1994.0</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="1">
+        <v>7.6697669E7</v>
+      </c>
+      <c r="I5" s="1">
+        <v>7.6697669E7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>14.0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1994.0</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1">
+        <v>7.6697669E7</v>
+      </c>
+      <c r="I6" s="1">
+        <v>7.6697669E7</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>